<commit_message>
changed config and dataxls relative paths to absolutepaths
</commit_message>
<xml_diff>
--- a/target/classes/com/mitthsb/qa/testdata/data.xlsx
+++ b/target/classes/com/mitthsb/qa/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pperla\eclipse-workspace\MittHSBTest\src\main\java\com\mitthsb\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B38F75-2A10-4AB1-9D29-C313452A83A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C68BE49-1B26-4390-9872-F7E4AD0B94AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>asd00asd!</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>192101031686</t>
+  </si>
+  <si>
+    <t>198806011642</t>
+  </si>
+  <si>
+    <t>198109231665</t>
   </si>
 </sst>
 </file>
@@ -86,8 +95,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,19 +379,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
@@ -390,10 +401,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>192101031686</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -401,10 +412,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>198806011642</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -412,10 +423,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>198109231665</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
@@ -423,10 +434,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>198109231665</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">

</xml_diff>